<commit_message>
At most one entity value match for the same synonym in a given entity
</commit_message>
<xml_diff>
--- a/dialogtool/internaltest/internaltest_results.xlsx
+++ b/dialogtool/internaltest/internaltest_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Laurent\OneDrive\Dev\Github\ConversationTools\dialogtool\bin\Debug\result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Laurent\OneDrive\Dev\Github\ConversationTools\dialogtool\internaltest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="406">
   <si>
     <t>Input</t>
   </si>
@@ -1780,7 +1780,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
+      <selection pane="bottomLeft" activeCell="O158" sqref="O158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5557,7 +5557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>198</v>
       </c>
@@ -5586,18 +5586,16 @@
       <c r="K84" t="s">
         <v>196</v>
       </c>
-      <c r="L84" t="s">
-        <v>202</v>
-      </c>
+      <c r="L84"/>
       <c r="M84"/>
       <c r="N84"/>
       <c r="O84" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>name65|name66||</v>
+        <v>name65|||</v>
       </c>
       <c r="P84" s="2" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -5723,7 +5721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>210</v>
       </c>
@@ -5752,18 +5750,16 @@
       <c r="K88" t="s">
         <v>212</v>
       </c>
-      <c r="L88" t="s">
-        <v>212</v>
-      </c>
+      <c r="L88"/>
       <c r="M88"/>
       <c r="N88"/>
       <c r="O88" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>name73|name73||</v>
+        <v>name73|||</v>
       </c>
       <c r="P88" s="2" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -5848,7 +5844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>220</v>
       </c>
@@ -5877,18 +5873,16 @@
       <c r="K91" t="s">
         <v>218</v>
       </c>
-      <c r="L91" t="s">
-        <v>224</v>
-      </c>
+      <c r="L91"/>
       <c r="M91"/>
       <c r="N91"/>
       <c r="O91" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>name75|name76||</v>
+        <v>name75|||</v>
       </c>
       <c r="P91" s="2" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improved error messages (bugs fixed in check command)
</commit_message>
<xml_diff>
--- a/dialogtool/internaltest/internaltest_results.xlsx
+++ b/dialogtool/internaltest/internaltest_results.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="406">
   <si>
     <t>Input</t>
   </si>
@@ -1780,7 +1780,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O158" sqref="O158"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7450,7 +7450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>315</v>
       </c>
@@ -7478,17 +7478,21 @@
       <c r="J131" t="s">
         <v>315</v>
       </c>
-      <c r="K131"/>
-      <c r="L131"/>
+      <c r="K131" t="s">
+        <v>313</v>
+      </c>
+      <c r="L131" t="s">
+        <v>313</v>
+      </c>
       <c r="M131"/>
       <c r="N131"/>
       <c r="O131" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>|||</v>
+        <v>name10|name10||</v>
       </c>
       <c r="P131" s="2" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7534,7 +7538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>321</v>
       </c>
@@ -7562,17 +7566,21 @@
       <c r="J133" t="s">
         <v>321</v>
       </c>
-      <c r="K133"/>
-      <c r="L133"/>
+      <c r="K133" t="s">
+        <v>319</v>
+      </c>
+      <c r="L133" t="s">
+        <v>319</v>
+      </c>
       <c r="M133"/>
       <c r="N133"/>
       <c r="O133" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>|||</v>
+        <v>name11|name11||</v>
       </c>
       <c r="P133" s="2" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reliable error message for Insurance dialog + metrics on the dialog file
</commit_message>
<xml_diff>
--- a/dialogtool/internaltest/internaltest_results.xlsx
+++ b/dialogtool/internaltest/internaltest_results.xlsx
@@ -1775,12 +1775,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G138" sqref="G138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1835,7 +1834,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1880,7 +1879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1925,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1962,7 +1961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -2007,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -2052,7 +2051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2105,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -2158,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -2211,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -2256,7 +2255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -2293,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -2330,7 +2329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -2375,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -2420,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
@@ -2526,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -2579,7 +2578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -2624,7 +2623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -2669,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -2706,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
@@ -2743,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>55</v>
       </c>
@@ -2788,7 +2787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>57</v>
       </c>
@@ -2833,7 +2832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>59</v>
       </c>
@@ -2886,7 +2885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>61</v>
       </c>
@@ -2939,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -2992,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>65</v>
       </c>
@@ -3037,7 +3036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>67</v>
       </c>
@@ -3082,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>69</v>
       </c>
@@ -3119,7 +3118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>71</v>
       </c>
@@ -3156,7 +3155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>73</v>
       </c>
@@ -3201,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>75</v>
       </c>
@@ -3246,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>77</v>
       </c>
@@ -3299,7 +3298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>79</v>
       </c>
@@ -3352,7 +3351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>81</v>
       </c>
@@ -3405,7 +3404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>83</v>
       </c>
@@ -3450,7 +3449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>88</v>
       </c>
@@ -3495,7 +3494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>90</v>
       </c>
@@ -3532,7 +3531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>92</v>
       </c>
@@ -3569,7 +3568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>94</v>
       </c>
@@ -3614,7 +3613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>96</v>
       </c>
@@ -3659,7 +3658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>98</v>
       </c>
@@ -3712,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>101</v>
       </c>
@@ -3765,7 +3764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>103</v>
       </c>
@@ -3818,7 +3817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>105</v>
       </c>
@@ -3863,7 +3862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>107</v>
       </c>
@@ -3908,7 +3907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>109</v>
       </c>
@@ -3945,7 +3944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>111</v>
       </c>
@@ -3982,7 +3981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>113</v>
       </c>
@@ -4027,7 +4026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>115</v>
       </c>
@@ -4072,7 +4071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>117</v>
       </c>
@@ -4125,7 +4124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>119</v>
       </c>
@@ -4178,7 +4177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>121</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>123</v>
       </c>
@@ -4276,7 +4275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>128</v>
       </c>
@@ -4321,7 +4320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>130</v>
       </c>
@@ -4358,7 +4357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>132</v>
       </c>
@@ -4395,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>134</v>
       </c>
@@ -4440,7 +4439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>136</v>
       </c>
@@ -4485,7 +4484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>138</v>
       </c>
@@ -4538,7 +4537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>141</v>
       </c>
@@ -4591,7 +4590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>143</v>
       </c>
@@ -4644,7 +4643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>145</v>
       </c>
@@ -4689,7 +4688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>147</v>
       </c>
@@ -4734,7 +4733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>149</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>151</v>
       </c>
@@ -4808,7 +4807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>153</v>
       </c>
@@ -4853,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>155</v>
       </c>
@@ -4898,7 +4897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>157</v>
       </c>
@@ -4951,7 +4950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>159</v>
       </c>
@@ -5004,7 +5003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>161</v>
       </c>
@@ -5057,7 +5056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>163</v>
       </c>
@@ -5098,7 +5097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>167</v>
       </c>
@@ -5139,7 +5138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>169</v>
       </c>
@@ -5184,7 +5183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>172</v>
       </c>
@@ -5229,7 +5228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>174</v>
       </c>
@@ -5270,7 +5269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>178</v>
       </c>
@@ -5311,7 +5310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>182</v>
       </c>
@@ -5352,7 +5351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>186</v>
       </c>
@@ -5393,7 +5392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>188</v>
       </c>
@@ -5434,7 +5433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>190</v>
       </c>
@@ -5475,7 +5474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>192</v>
       </c>
@@ -5516,7 +5515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>194</v>
       </c>
@@ -5557,7 +5556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>198</v>
       </c>
@@ -5598,7 +5597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>200</v>
       </c>
@@ -5639,7 +5638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>204</v>
       </c>
@@ -5680,7 +5679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>208</v>
       </c>
@@ -5721,7 +5720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>210</v>
       </c>
@@ -5762,7 +5761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>214</v>
       </c>
@@ -5803,7 +5802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>216</v>
       </c>
@@ -5844,7 +5843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>220</v>
       </c>
@@ -5885,7 +5884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>222</v>
       </c>
@@ -5926,7 +5925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>226</v>
       </c>
@@ -5967,7 +5966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>230</v>
       </c>
@@ -6008,7 +6007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>232</v>
       </c>
@@ -6049,7 +6048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>234</v>
       </c>
@@ -6090,7 +6089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>236</v>
       </c>
@@ -6131,7 +6130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>240</v>
       </c>
@@ -6172,7 +6171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>242</v>
       </c>
@@ -6213,7 +6212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>244</v>
       </c>
@@ -6254,7 +6253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>246</v>
       </c>
@@ -6295,7 +6294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>250</v>
       </c>
@@ -6336,7 +6335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>252</v>
       </c>
@@ -6377,7 +6376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>254</v>
       </c>
@@ -6418,7 +6417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>256</v>
       </c>
@@ -6459,7 +6458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>260</v>
       </c>
@@ -6500,7 +6499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>262</v>
       </c>
@@ -6541,7 +6540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>264</v>
       </c>
@@ -6582,7 +6581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>266</v>
       </c>
@@ -6623,7 +6622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>270</v>
       </c>
@@ -6664,7 +6663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>272</v>
       </c>
@@ -6705,7 +6704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>274</v>
       </c>
@@ -6746,7 +6745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>402</v>
       </c>
@@ -6776,8 +6775,12 @@
         <f t="shared" si="4"/>
         <v>name91|||</v>
       </c>
-    </row>
-    <row r="114" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P113" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>403</v>
       </c>
@@ -6807,8 +6810,12 @@
         <f t="shared" si="4"/>
         <v>name91|||</v>
       </c>
-    </row>
-    <row r="115" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P114" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>276</v>
       </c>
@@ -6849,7 +6856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>280</v>
       </c>
@@ -6890,7 +6897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>282</v>
       </c>
@@ -6931,7 +6938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>284</v>
       </c>
@@ -6972,7 +6979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>404</v>
       </c>
@@ -7002,8 +7009,12 @@
         <f t="shared" si="4"/>
         <v>name92|||</v>
       </c>
-    </row>
-    <row r="120" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P119" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>405</v>
       </c>
@@ -7033,8 +7044,12 @@
         <f t="shared" si="4"/>
         <v>name92|||</v>
       </c>
-    </row>
-    <row r="121" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P120" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>286</v>
       </c>
@@ -7075,7 +7090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>290</v>
       </c>
@@ -7116,7 +7131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>292</v>
       </c>
@@ -7157,7 +7172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>294</v>
       </c>
@@ -7198,7 +7213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>296</v>
       </c>
@@ -7239,7 +7254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>300</v>
       </c>
@@ -7280,7 +7295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>302</v>
       </c>
@@ -7321,7 +7336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>304</v>
       </c>
@@ -7362,7 +7377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>306</v>
       </c>
@@ -7450,7 +7465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>315</v>
       </c>
@@ -7538,7 +7553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>321</v>
       </c>
@@ -7583,7 +7598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>323</v>
       </c>
@@ -7624,7 +7639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>327</v>
       </c>
@@ -7665,7 +7680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>331</v>
       </c>
@@ -7706,7 +7721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>335</v>
       </c>
@@ -7751,7 +7766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>338</v>
       </c>
@@ -7792,7 +7807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>340</v>
       </c>
@@ -7833,7 +7848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>342</v>
       </c>
@@ -7874,7 +7889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>346</v>
       </c>
@@ -7915,7 +7930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>350</v>
       </c>
@@ -7956,7 +7971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>354</v>
       </c>
@@ -8001,7 +8016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>357</v>
       </c>
@@ -8042,7 +8057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>361</v>
       </c>
@@ -8083,7 +8098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>365</v>
       </c>
@@ -8124,7 +8139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>369</v>
       </c>
@@ -8165,7 +8180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>371</v>
       </c>
@@ -8206,7 +8221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>373</v>
       </c>
@@ -8251,7 +8266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>376</v>
       </c>
@@ -8292,7 +8307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>380</v>
       </c>
@@ -8333,7 +8348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>384</v>
       </c>
@@ -8374,7 +8389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:16" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>388</v>
       </c>
@@ -8420,13 +8435,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="P1:P153">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="FAUX"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="P1:P153"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated concept synonyms and entity value string comparisons to match the latest tests donc with Dialog and the indications of the labs
</commit_message>
<xml_diff>
--- a/dialogtool/internaltest/internaltest_results.xlsx
+++ b/dialogtool/internaltest/internaltest_results.xlsx
@@ -1778,8 +1778,8 @@
   <dimension ref="A1:P153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G138" sqref="G138"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>